<commit_message>
FIXME: chart title updated
</commit_message>
<xml_diff>
--- a/doc/kretprobe scalability.xlsx
+++ b/doc/kretprobe scalability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8CEF2AC-E983-E342-AB56-EEBDBE00BD60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C28A60C-62B3-754D-96A7-10CED98C8DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60160" yWindow="-6540" windowWidth="60160" windowHeight="33840" xr2:uid="{B0F7ECFE-305D-2349-A24A-1A6269EF7B35}"/>
+    <workbookView xWindow="-58840" yWindow="-6040" windowWidth="60160" windowHeight="33380" activeTab="1" xr2:uid="{B0F7ECFE-305D-2349-A24A-1A6269EF7B35}"/>
   </bookViews>
   <sheets>
     <sheet name="kretprobe" sheetId="1" r:id="rId1"/>
@@ -2177,7 +2177,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$280:$N$280</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>17233640</c:v>
@@ -2203,7 +2203,7 @@
                 <c:pt idx="7">
                   <c:v>3382013</c:v>
                 </c:pt>
-                <c:pt idx="8" formatCode="General">
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
@@ -2312,7 +2312,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$281:$N$281</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>18458229</c:v>
@@ -2447,7 +2447,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$282:$N$282</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>19360905</c:v>
@@ -2582,7 +2582,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$283:$N$283</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>17556183</c:v>
@@ -2717,7 +2717,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$284:$N$284</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>18302399</c:v>
@@ -2852,7 +2852,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$285:$N$285</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>19221965</c:v>
@@ -2993,7 +2993,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$286:$N$286</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>17555121</c:v>
@@ -3134,7 +3134,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$287:$N$287</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>18710480</c:v>
@@ -3275,7 +3275,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$288:$N$288</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>18800528</c:v>
@@ -3416,7 +3416,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$289:$N$289</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>17275601</c:v>
@@ -3557,7 +3557,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$290:$N$290</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>18742147</c:v>
@@ -3698,7 +3698,7 @@
             <c:numRef>
               <c:f>[1]Extreme!$C$291:$N$291</c:f>
               <c:numCache>
-                <c:formatCode>#,##0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>18525938</c:v>
@@ -3831,7 +3831,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4069,8 +4069,8 @@
             <c:strRef>
               <c:f>[1]Extreme!$A$5:$B$5</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>zigzag:max=96</c:v>
                 </c:pt>
               </c:strCache>
@@ -4210,8 +4210,8 @@
             <c:strRef>
               <c:f>[1]Extreme!$A$6:$B$6</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>freelist:max=96</c:v>
                 </c:pt>
               </c:strCache>
@@ -4351,8 +4351,8 @@
             <c:strRef>
               <c:f>[1]Extreme!$A$7:$B$7</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>array:max=96</c:v>
                 </c:pt>
               </c:strCache>
@@ -4492,8 +4492,8 @@
             <c:strRef>
               <c:f>[1]Extreme!$A$8:$B$8</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>strided:max=96</c:v>
                 </c:pt>
               </c:strCache>
@@ -4633,8 +4633,8 @@
             <c:strRef>
               <c:f>[1]Extreme!$A$9:$B$9</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>zigzag:max=192</c:v>
                 </c:pt>
               </c:strCache>
@@ -4774,8 +4774,8 @@
             <c:strRef>
               <c:f>[1]Extreme!$A$10:$B$10</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>freelist:max=192</c:v>
                 </c:pt>
               </c:strCache>
@@ -4915,8 +4915,8 @@
             <c:strRef>
               <c:f>[1]Extreme!$A$11:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>array:max=192</c:v>
                 </c:pt>
               </c:strCache>
@@ -5062,8 +5062,8 @@
             <c:strRef>
               <c:f>[1]Extreme!$A$12:$B$12</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="1">
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
                   <c:v>strided:max=192</c:v>
                 </c:pt>
               </c:strCache>
@@ -6946,41 +6946,6 @@
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
-          <a:p>
-            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-              <a:lnSpc>
-                <a:spcPct val="100000"/>
-              </a:lnSpc>
-              <a:spcBef>
-                <a:spcPts val="0"/>
-              </a:spcBef>
-              <a:spcAft>
-                <a:spcPts val="0"/>
-              </a:spcAft>
-              <a:buClrTx/>
-              <a:buSzTx/>
-              <a:buFontTx/>
-              <a:buNone/>
-              <a:tabLst/>
-              <a:defRPr>
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>(with 1us delay before insertion back)</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CN">
-              <a:effectLst/>
-            </a:endParaRPr>
-          </a:p>
         </c:rich>
       </c:tx>
       <c:layout>
@@ -8149,13 +8114,27 @@
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr algn="ctr" rtl="0">
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
               <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
+                  <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  </a:sysClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -8169,10 +8148,42 @@
             <a:endParaRPr lang="en-CN"/>
           </a:p>
           <a:p>
-            <a:pPr algn="ctr" rtl="0">
-              <a:defRPr/>
+            <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>(with 1us delay before insertion back)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CN">
+              <a:effectLst/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -8196,13 +8207,27 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr algn="ctr" rtl="0">
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
             <a:defRPr sz="1920" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
+                <a:sysClr val="windowText" lastClr="000000">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
-                </a:schemeClr>
+                </a:sysClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -15949,7 +15974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D4BB04F-22A3-1D48-A1DB-0FCE1C1F1BBB}">
   <dimension ref="B3:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A45" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -16944,8 +16969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D084A7CC-3B35-1F49-A72B-EFEC83C59514}">
   <dimension ref="B2:O216"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A274" sqref="A200:XFD274"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="L141" sqref="L141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>